<commit_message>
added automatic folder creation for non existing folders in scriptRng, arg, res and diag fixed bug with #REF! in R_Addin names
</commit_message>
<xml_diff>
--- a/test/testRAddin.xlsx
+++ b/test/testRAddin.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\RAddin\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBDE66E4-011F-487D-9B25-2FA3373D72B1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1470" windowWidth="18795" windowHeight="7830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="1470" windowWidth="18795" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -31,6 +25,7 @@
     <definedName name="R_AddinAnotherDef" localSheetId="2">Test_OtherSheet!$J$7:$L$12</definedName>
     <definedName name="R_AddinAnotherDef">'Main Test'!$M$1:$O$5</definedName>
     <definedName name="R_AddinErrorInDef">'Main Test'!$P$1:$R$5</definedName>
+    <definedName name="R_AddinNewResDiagDir">'Main Test'!$S$1:$U$5</definedName>
     <definedName name="R_AddinOtherPlot">Test_RdotNet!$A$39:$C$40</definedName>
     <definedName name="R_AddinScriptCell" localSheetId="1">Test_scriptRng!$A$25:$C$29</definedName>
     <definedName name="R_AddinScriptRange" localSheetId="1">Test_scriptRng!$A$19:$C$23</definedName>
@@ -47,7 +42,7 @@
     <definedName name="testdiagram" localSheetId="1">Test_scriptRng!$D$2</definedName>
     <definedName name="testdiagram">'Main Test'!$J$8</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -60,30 +55,44 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="test_out" type="6" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="test_out" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="test_out1" type="6" refreshedVersion="0" background="1">
+  <connection id="2" name="test_out1" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="test_out2" type="6" refreshedVersion="0" background="1">
+  <connection id="3" name="test_out2" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="test_out3" type="6" refreshedVersion="0" background="1">
+  <connection id="4" name="test_out3" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\\test_out.txt" decimal="," thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="test_out4" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" name="test_out5" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
@@ -93,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1944" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1957" uniqueCount="65">
   <si>
     <t/>
   </si>
@@ -320,7 +329,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="\."/>
@@ -490,12 +499,12 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Komma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Prozent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Komma 2" xfId="3"/>
+    <cellStyle name="Prozent 2" xfId="4"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Standard 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Standard 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Standard 2" xfId="1"/>
+    <cellStyle name="Standard 2 2" xfId="5"/>
+    <cellStyle name="Standard 3" xfId="2"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -522,7 +531,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -547,61 +556,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="testdiagram.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2676525" y="1133475"/>
-          <a:ext cx="4572000" cy="4572000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -618,7 +572,7 @@
         <xdr:cNvPr id="3" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F09DEF9E-034B-4BEF-88DD-83D730E1015E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F09DEF9E-034B-4BEF-88DD-83D730E1015E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -653,7 +607,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -673,7 +627,7 @@
         <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -708,7 +662,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -728,7 +682,7 @@
         <xdr:cNvPr id="11" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -764,9 +718,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -804,9 +758,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -839,26 +793,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -891,26 +828,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1083,12 +1003,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="eingabe"/>
-  <dimension ref="A1:R50"/>
+  <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="P1" sqref="P1:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1099,7 +1019,7 @@
     <col min="18" max="18" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B1" s="11" t="s">
         <v>14</v>
       </c>
@@ -1132,17 +1052,24 @@
       </c>
       <c r="N1" t="str">
         <f ca="1">SUBSTITUTE(CELL("DATEINAME",O1),"[testRAddin.xlsx]Main Test","")</f>
-        <v>C:\dev\RAddin\test\</v>
+        <v>C:\dev\RAddin\trunk\test\</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="Q1" t="str">
         <f ca="1">SUBSTITUTE(CELL("DATEINAME",R1),"[testRAddin.xlsx]Main Test","")</f>
-        <v>C:\dev\RAddin\test\</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+        <v>C:\dev\RAddin\trunk\test\</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="T1" t="str">
+        <f ca="1">SUBSTITUTE(CELL("DATEINAME",U1),"[testRAddin.xlsx]Main Test","")</f>
+        <v>C:\dev\RAddin\trunk\test\</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="11">
         <v>0.29749999999999999</v>
       </c>
@@ -1192,8 +1119,17 @@
       <c r="R2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>0.30690000000000001</v>
       </c>
@@ -1243,8 +1179,17 @@
       <c r="R3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>1.04E-2</v>
       </c>
@@ -1294,8 +1239,17 @@
       <c r="R4" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" t="s">
+        <v>10</v>
+      </c>
+      <c r="U4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>5.1000000000000004E-3</v>
       </c>
@@ -1345,8 +1299,17 @@
       <c r="R5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="S5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="T5" t="s">
+        <v>4</v>
+      </c>
+      <c r="U5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>0.21249999999999999</v>
       </c>
@@ -1376,7 +1339,7 @@
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>5.4999999999999997E-3</v>
       </c>
@@ -1406,7 +1369,7 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>8.5000000000000006E-3</v>
       </c>
@@ -1436,7 +1399,7 @@
       <c r="L8" s="7"/>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>1.1900000000000001E-2</v>
       </c>
@@ -1466,7 +1429,7 @@
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>2.3E-2</v>
       </c>
@@ -1496,7 +1459,7 @@
       <c r="L10" s="7"/>
       <c r="M10" s="7"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>0.3836</v>
       </c>
@@ -1526,7 +1489,7 @@
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>0.34520000000000001</v>
       </c>
@@ -1556,7 +1519,7 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>1.4500000000000001E-2</v>
       </c>
@@ -1586,7 +1549,7 @@
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>1.4500000000000001E-2</v>
       </c>
@@ -1616,7 +1579,7 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>1.0200000000000001E-2</v>
       </c>
@@ -1646,7 +1609,7 @@
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>0.29749999999999999</v>
       </c>
@@ -2601,16 +2564,16 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;Z&amp;F&amp;A</oddFooter>
   </headerFooter>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M302"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:C29"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9065,12 +9028,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="eingabeToy"/>
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J7" sqref="J7:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9400,7 +9363,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Fehler im scriptcheck behoben
</commit_message>
<xml_diff>
--- a/test/testRAddin.xlsx
+++ b/test/testRAddin.xlsx
@@ -551,6 +551,55 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="testdiagram.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676525" y="1133475"/>
+          <a:ext cx="4572000" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -567,7 +616,7 @@
         <xdr:cNvPr id="3" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F09DEF9E-034B-4BEF-88DD-83D730E1015E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F09DEF9E-034B-4BEF-88DD-83D730E1015E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -602,7 +651,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -622,7 +671,7 @@
         <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -657,7 +706,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -677,7 +726,7 @@
         <xdr:cNvPr id="11" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-00000B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1236,7 +1285,7 @@
       </c>
       <c r="U4" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>20190528</v>
+        <v>unterverz/unterunterverz/20190528</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -1297,7 +1346,7 @@
       </c>
       <c r="U5" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>20190528</v>
+        <v>unterverz/unterunterverz/20190528</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -1360,8 +1409,8 @@
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
       <c r="U7" s="22" t="str">
-        <f ca="1">TEXT(TODAY(),"JJJJMMTT")</f>
-        <v>20190528</v>
+        <f ca="1">"unterverz/unterunterverz/"&amp;TEXT(TODAY(),"JJJJMMTT")</f>
+        <v>unterverz/unterunterverz/20190528</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -2559,6 +2608,7 @@
   <headerFooter alignWithMargins="0">
     <oddFooter>&amp;L&amp;Z&amp;F&amp;A</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2716,7 +2766,7 @@
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="str">
         <f ca="1">"write.table(test_in[,1],file="""&amp;variablesVerzeichnis&amp;"/test_out.txt"",sep=""\t"",row.names=FALSE,col.names=FALSE,quote=FALSE)"</f>
-        <v>write.table(test_in[,1],file="20190528/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
+        <v>write.table(test_in[,1],file="unterverz/unterunterverz/20190528/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -2739,7 +2789,7 @@
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="9" t="str">
         <f ca="1">"png(filename="""&amp;variablesVerzeichnis&amp;"/testdiagram.png"")"</f>
-        <v>png(filename="20190528/testdiagram.png")</v>
+        <v>png(filename="unterverz/unterunterverz/20190528/testdiagram.png")</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>

</xml_diff>

<commit_message>
upgraded exceldna upgraded RDotNet Added refreshRDefinitions Button to AboutBox
</commit_message>
<xml_diff>
--- a/test/testRAddin.xlsx
+++ b/test/testRAddin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1470" windowWidth="18795" windowHeight="7830"/>
+    <workbookView xWindow="1380" yWindow="1470" windowWidth="18795" windowHeight="7830" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -277,16 +277,6 @@
     <t>argc</t>
   </si>
   <si>
-    <t>library(ggplot2)
-test_out &lt;- as.Date(c("2017-01-01","2017-01-02","2017-01-03"))+25569 # difference between 1/1/1900 and 1/1/1970 + MS error
-test_out2 &lt;- test_in
-rownames(test_out2) &lt;- c("huey","dewey","louie")
-gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
-png(filename="C:/dev/Raddin/trunk/testdiagram.png")
-print(gplot)
-dev.off()</t>
-  </si>
-  <si>
     <t>huey</t>
   </si>
   <si>
@@ -302,13 +292,6 @@
     <t>ret</t>
   </si>
   <si>
-    <t>library(ggplot2)
-gplot &lt;- ggplot(data = test_in, aes(x = in6, y = in7) ) + geom_point()
-png(filename="C:/dev/Raddin/trunk/testdiagram.png")
-print(gplot)
-dev.off()</t>
-  </si>
-  <si>
     <t>ä</t>
   </si>
   <si>
@@ -319,6 +302,23 @@
   </si>
   <si>
     <t>-&gt; Attention, diagram for test_scriptcell appears in Main Test !!!</t>
+  </si>
+  <si>
+    <t>library(ggplot2)
+gplot &lt;- ggplot(data = test_in, aes(x = in6, y = in7) ) + geom_point()
+png(filename="C:/dev/Raddin/trunk/test/testdiagram.png")
+print(gplot)
+dev.off()</t>
+  </si>
+  <si>
+    <t>library(ggplot2)
+test_out &lt;- as.Date(c("2017-01-01","2017-01-02","2017-01-03"))+25569 # difference between 1/1/1900 and 1/1/1970 + MS error
+test_out2 &lt;- test_in
+rownames(test_out2) &lt;- c("huey","dewey","louie")
+gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
+png(filename="C:/dev/Raddin/trunk/test/testdiagram.png")
+print(gplot)
+dev.off()</t>
   </si>
 </sst>
 </file>
@@ -616,7 +616,7 @@
         <xdr:cNvPr id="3" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F09DEF9E-034B-4BEF-88DD-83D730E1015E}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F09DEF9E-034B-4BEF-88DD-83D730E1015E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -671,7 +671,7 @@
         <xdr:cNvPr id="10" name="testdiagram.png">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -723,13 +723,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="11" name="testdiagram.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-00000B000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1051,7 +1045,7 @@
   <sheetPr codeName="eingabe"/>
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="S1" sqref="S1:U5"/>
     </sheetView>
   </sheetViews>
@@ -1285,7 +1279,7 @@
       </c>
       <c r="U4" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20190528</v>
+        <v>unterverz/unterunterverz/20190726</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -1346,7 +1340,7 @@
       </c>
       <c r="U5" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20190528</v>
+        <v>unterverz/unterunterverz/20190726</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -1410,7 +1404,7 @@
       <c r="M7" s="7"/>
       <c r="U7" s="22" t="str">
         <f ca="1">"unterverz/unterunterverz/"&amp;TEXT(TODAY(),"JJJJMMTT")</f>
-        <v>unterverz/unterunterverz/20190528</v>
+        <v>unterverz/unterunterverz/20190726</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -2586,13 +2580,13 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I48" s="7"/>
     </row>
@@ -2766,7 +2760,7 @@
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="str">
         <f ca="1">"write.table(test_in[,1],file="""&amp;variablesVerzeichnis&amp;"/test_out.txt"",sep=""\t"",row.names=FALSE,col.names=FALSE,quote=FALSE)"</f>
-        <v>write.table(test_in[,1],file="unterverz/unterunterverz/20190528/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
+        <v>write.table(test_in[,1],file="unterverz/unterunterverz/20190726/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -2789,7 +2783,7 @@
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="9" t="str">
         <f ca="1">"png(filename="""&amp;variablesVerzeichnis&amp;"/testdiagram.png"")"</f>
-        <v>png(filename="unterverz/unterunterverz/20190528/testdiagram.png")</v>
+        <v>png(filename="unterverz/unterunterverz/20190726/testdiagram.png")</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
@@ -2982,7 +2976,7 @@
     <row r="30" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30" s="24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
@@ -9414,8 +9408,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9431,7 +9425,7 @@
         <v>50</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>21</v>
@@ -9481,7 +9475,7 @@
         <v>0.1</v>
       </c>
       <c r="I2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J2" s="1">
         <v>3</v>
@@ -9513,7 +9507,7 @@
         <v>0.8</v>
       </c>
       <c r="I3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J3" s="1">
         <v>3</v>
@@ -9545,7 +9539,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J4" s="1">
         <v>3</v>
@@ -9587,7 +9581,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -9602,7 +9596,7 @@
         <v>0.1</v>
       </c>
       <c r="J9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -9613,7 +9607,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10">
         <v>68.56</v>
@@ -9628,7 +9622,7 @@
         <v>0.8</v>
       </c>
       <c r="J10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K10" s="22">
         <v>3</v>
@@ -9639,7 +9633,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11">
         <v>300</v>
@@ -9654,7 +9648,7 @@
         <v>5</v>
       </c>
       <c r="J11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K11" s="22">
         <v>3</v>
@@ -9671,7 +9665,7 @@
         <v>50</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
documentation update (also API doc works now)
</commit_message>
<xml_diff>
--- a/test/testRAddin.xlsx
+++ b/test/testRAddin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1470" windowWidth="18795" windowHeight="7830" activeTab="3"/>
+    <workbookView xWindow="1380" yWindow="1470" windowWidth="18795" windowHeight="7830" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -78,22 +78,43 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="test_out3" type="6" refreshedVersion="0" background="1">
+  <connection id="4" name="test_out21" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\\test_out2.txt" decimal="," thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="test_out3" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="test_out4" type="6" refreshedVersion="0" background="1">
+  <connection id="6" name="test_out4" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="test_out5" type="6" refreshedVersion="0" background="1">
+  <connection id="7" name="test_out5" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" name="test_out6" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\\test_out.txt" decimal="," thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" name="test_out7" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
@@ -103,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="64">
   <si>
     <t/>
   </si>
@@ -160,9 +181,6 @@
   </si>
   <si>
     <t>rexec</t>
-  </si>
-  <si>
-    <t>cmd</t>
   </si>
   <si>
     <t>testStartRscript.cmd</t>
@@ -304,18 +322,26 @@
     <t>-&gt; Attention, diagram for test_scriptcell appears in Main Test !!!</t>
   </si>
   <si>
-    <t>library(ggplot2)
-gplot &lt;- ggplot(data = test_in, aes(x = in6, y = in7) ) + geom_point()
+    <t>cmd.exe</t>
+  </si>
+  <si>
+    <t>/c</t>
+  </si>
+  <si>
+    <t># cannot be called via shell, because test_in is not read from file -&gt; in memory !!
+library(ggplot2)
+test_out &lt;- as.Date(c("2017-01-01","2017-01-02","2017-01-03"))+25569 # difference between 1/1/1900 and 1/1/1970 + MS error
+test_out2 &lt;- test_in
+rownames(test_out2) &lt;- c("huey","dewey","louie")
+gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
 png(filename="C:/dev/Raddin/trunk/test/testdiagram.png")
 print(gplot)
 dev.off()</t>
   </si>
   <si>
-    <t>library(ggplot2)
-test_out &lt;- as.Date(c("2017-01-01","2017-01-02","2017-01-03"))+25569 # difference between 1/1/1900 and 1/1/1970 + MS error
-test_out2 &lt;- test_in
-rownames(test_out2) &lt;- c("huey","dewey","louie")
-gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
+    <t># cannot be called via shell, because test_in is not read from file -&gt; in memory !!
+library(ggplot2)
+gplot &lt;- ggplot(data = test_in, aes(x = in6, y = in7) ) + geom_point()
 png(filename="C:/dev/Raddin/trunk/test/testdiagram.png")
 print(gplot)
 dev.off()</t>
@@ -564,7 +590,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="testdiagram.png"/>
+        <xdr:cNvPr id="9" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -613,13 +639,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="testdiagram.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F09DEF9E-034B-4BEF-88DD-83D730E1015E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -668,13 +688,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="testdiagram.png">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CEE521C-90CF-430D-A30C-846F8D1C58A3}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -693,7 +707,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3114675" y="2590800"/>
+          <a:off x="2609850" y="2590800"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -723,7 +737,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="testdiagram.png"/>
+        <xdr:cNvPr id="5" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -742,7 +756,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="2305050"/>
+          <a:off x="0" y="2409825"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1046,7 +1060,7 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:U5"/>
+      <selection activeCell="U4" sqref="U4:U5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1146,7 +1160,7 @@
         <v>8</v>
       </c>
       <c r="O2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>1</v>
@@ -1155,13 +1169,13 @@
         <v>8</v>
       </c>
       <c r="R2" t="s">
+        <v>47</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="T2" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -1203,7 +1217,7 @@
         <v>9</v>
       </c>
       <c r="O3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>6</v>
@@ -1212,7 +1226,7 @@
         <v>9</v>
       </c>
       <c r="R3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>6</v>
@@ -1260,7 +1274,7 @@
         <v>10</v>
       </c>
       <c r="O4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>5</v>
@@ -1269,7 +1283,7 @@
         <v>10</v>
       </c>
       <c r="R4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>5</v>
@@ -1321,7 +1335,7 @@
         <v>4</v>
       </c>
       <c r="O5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>7</v>
@@ -1330,7 +1344,7 @@
         <v>4</v>
       </c>
       <c r="R5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>7</v>
@@ -2580,13 +2594,13 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I48" s="7"/>
     </row>
@@ -2611,8 +2625,8 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M302"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2627,7 +2641,7 @@
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B1" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1"/>
       <c r="D1"/>
@@ -2638,7 +2652,7 @@
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
@@ -2649,7 +2663,7 @@
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3"/>
       <c r="D3"/>
@@ -2660,7 +2674,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4"/>
       <c r="D4"/>
@@ -2671,7 +2685,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2682,7 +2696,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -2693,7 +2707,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -2704,7 +2718,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2715,7 +2729,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -2726,7 +2740,7 @@
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -2737,7 +2751,7 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -2748,7 +2762,7 @@
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -2771,7 +2785,7 @@
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14"/>
       <c r="D14"/>
@@ -2794,7 +2808,7 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -2805,7 +2819,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -2840,10 +2854,10 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C20"/>
       <c r="D20"/>
@@ -2873,7 +2887,10 @@
       <c r="B22" t="s">
         <v>10</v>
       </c>
-      <c r="C22"/>
+      <c r="C22" t="str">
+        <f ca="1">variablesVerzeichnis</f>
+        <v>unterverz/unterunterverz/20190726</v>
+      </c>
       <c r="D22"/>
       <c r="E22"/>
       <c r="F22"/>
@@ -2885,9 +2902,12 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23"/>
+        <v>38</v>
+      </c>
+      <c r="C23" t="str">
+        <f ca="1">variablesVerzeichnis</f>
+        <v>unterverz/unterunterverz/20190726</v>
+      </c>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
@@ -2920,10 +2940,10 @@
     </row>
     <row r="26" spans="1:8" ht="216.75" x14ac:dyDescent="0.2">
       <c r="A26" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C26"/>
       <c r="E26"/>
@@ -2976,7 +2996,7 @@
     <row r="30" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30" s="24" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30"/>
       <c r="D30"/>
@@ -9071,15 +9091,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="eingabeToy"/>
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:L12"/>
+      <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2" style="5" customWidth="1"/>
     <col min="2" max="2" width="4" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="2" style="5" bestFit="1" customWidth="1"/>
@@ -9087,9 +9107,9 @@
     <col min="9" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>14</v>
@@ -9120,7 +9140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9153,7 +9173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9184,10 +9204,10 @@
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9217,31 +9237,34 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="J5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="J7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="L7" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="C8" s="6"/>
       <c r="J8" s="4" t="s">
@@ -9251,53 +9274,53 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="J9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="J10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="J11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="J12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -9408,8 +9431,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39:C40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9420,15 +9443,15 @@
     <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="105" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>62</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>14</v>
@@ -9454,10 +9477,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D2">
         <v>42736</v>
@@ -9475,7 +9498,7 @@
         <v>0.1</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J2" s="1">
         <v>3</v>
@@ -9489,7 +9512,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3">
         <v>42737</v>
@@ -9507,7 +9530,7 @@
         <v>0.8</v>
       </c>
       <c r="I3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J3" s="1">
         <v>3</v>
@@ -9521,7 +9544,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4">
         <v>42738</v>
@@ -9539,7 +9562,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="J4" s="1">
         <v>3</v>
@@ -9553,7 +9576,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -9581,7 +9604,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -9596,7 +9619,7 @@
         <v>0.1</v>
       </c>
       <c r="J9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -9607,7 +9630,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10">
         <v>68.56</v>
@@ -9622,7 +9645,7 @@
         <v>0.8</v>
       </c>
       <c r="J10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K10" s="22">
         <v>3</v>
@@ -9633,7 +9656,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F11">
         <v>300</v>
@@ -9648,7 +9671,7 @@
         <v>5</v>
       </c>
       <c r="J11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K11" s="22">
         <v>3</v>
@@ -9660,12 +9683,12 @@
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="K12" s="21"/>
     </row>
-    <row r="39" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -9673,7 +9696,7 @@
         <v>7</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added trace messages improved r.net invocation debugging/interaction fixed dynamic graphics problem with r.net invocation
</commit_message>
<xml_diff>
--- a/test/testRAddin.xlsx
+++ b/test/testRAddin.xlsx
@@ -26,10 +26,10 @@
     <definedName name="R_AddinAnotherDef">'Main Test'!$M$1:$O$5</definedName>
     <definedName name="R_AddinErrorInDef">'Main Test'!$P$1:$R$5</definedName>
     <definedName name="R_AddinNewResDiagDir">'Main Test'!$S$1:$U$5</definedName>
-    <definedName name="R_AddinOtherPlot">Test_RdotNet!$A$39:$C$40</definedName>
-    <definedName name="R_AddinScriptCell" localSheetId="1">Test_scriptRng!$A$25:$C$29</definedName>
-    <definedName name="R_AddinScriptRange" localSheetId="1">Test_scriptRng!$A$19:$C$23</definedName>
-    <definedName name="scriptRange" localSheetId="1">Test_scriptRng!$B$1:$B$17</definedName>
+    <definedName name="R_AddinOtherPlot">Test_RdotNet!$A$39:$C$41</definedName>
+    <definedName name="R_AddinScriptCell" localSheetId="1">Test_scriptRng!$A$21:$C$25</definedName>
+    <definedName name="R_AddinScriptRange" localSheetId="1">Test_scriptRng!$A$15:$C$19</definedName>
+    <definedName name="scriptRange" localSheetId="1">Test_scriptRng!$B$1:$B$13</definedName>
     <definedName name="test_in" localSheetId="2">Test_OtherSheet!$B$1:$H$4</definedName>
     <definedName name="test_in" localSheetId="3">Test_RdotNet!$E$1:$K$4</definedName>
     <definedName name="test_in">'Main Test'!$B$1:$H$301</definedName>
@@ -71,49 +71,70 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="test_out2" type="6" refreshedVersion="0" background="1">
+  <connection id="3" name="test_out10" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="test_out2" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="test_out21" type="6" refreshedVersion="0" background="1">
+  <connection id="5" name="test_out21" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\\test_out2.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="test_out3" type="6" refreshedVersion="0" background="1">
+  <connection id="6" name="test_out3" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="test_out4" type="6" refreshedVersion="0" background="1">
+  <connection id="7" name="test_out4" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="test_out5" type="6" refreshedVersion="0" background="1">
+  <connection id="8" name="test_out5" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="test_out6" type="6" refreshedVersion="0" background="1">
+  <connection id="9" name="test_out6" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="test_out7" type="6" refreshedVersion="0" background="1">
+  <connection id="10" name="test_out7" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="11" name="test_out8" type="6" refreshedVersion="0" background="1">
+    <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="12" name="test_out9" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
@@ -124,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1952" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="60">
   <si>
     <t/>
   </si>
@@ -204,28 +225,7 @@
     <t>script.basename &lt;- dirname(script.name)</t>
   </si>
   <si>
-    <t>if (length(script.basename) == 0) {</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  # this only works RGui</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  script.basename &lt;- getSrcDirectory(function(x) {x})</t>
-  </si>
-  <si>
     <t>}</t>
-  </si>
-  <si>
-    <t>setwd(script.basename)</t>
-  </si>
-  <si>
-    <t>#test_in &lt;-as.matrix(read.csv2("test_in.txt",sep="\t",header=FALSE))</t>
-  </si>
-  <si>
-    <t>#mode(test_in) &lt;-"numeric"</t>
-  </si>
-  <si>
-    <t>test_in &lt;- read.csv2("test_in.txt",dec=".",sep="\t",header=TRUE)</t>
   </si>
   <si>
     <t>gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()</t>
@@ -235,25 +235,6 @@
   </si>
   <si>
     <t>dev.off()</t>
-  </si>
-  <si>
-    <t>library(ggplot2)
-initial.options &lt;- commandArgs(trailingOnly = FALSE)
-script.name &lt;- sub("--file=", "", initial.options[grep("--file=", initial.options)])
-script.basename &lt;- dirname(script.name)
-if (length(script.basename) == 0) {
-  # this only works RGui
-  script.basename &lt;- getSrcDirectory(function(x) {x})
-}
-setwd(script.basename)
-#test_in &lt;-as.matrix(read.csv2("test_in.txt",sep="\t",header=FALSE))
-#mode(test_in) &lt;-"numeric"
-test_in &lt;- read.csv2("test_in.txt",dec=".",sep="\t",header=TRUE)
-write.table(test_in[,1],file="test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)
-gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
-png(filename="testdiagram.png")
-print(gplot)
-dev.off()</t>
   </si>
   <si>
     <t>Test_scriptRng!testdiagram</t>
@@ -343,6 +324,32 @@
 library(ggplot2)
 gplot &lt;- ggplot(data = test_in, aes(x = in6, y = in7) ) + geom_point()
 png(filename="C:/dev/Raddin/trunk/test/testdiagram.png")
+print(gplot)
+dev.off()</t>
+  </si>
+  <si>
+    <t>if (length(script.basename) &gt; 0) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  setwd(script.basename)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  test_in &lt;- read.csv2("test_in.txt",dec=".",sep="\t",header=TRUE)</t>
+  </si>
+  <si>
+    <t>library(ggplot2)
+initial.options &lt;- commandArgs(trailingOnly = FALSE)
+script.name &lt;- sub("--file=", "", initial.options[grep("--file=", initial.options)])
+script.basename &lt;- dirname(script.name)
+if (length(script.basename) &gt; 0) {
+   setwd(script.basename)
+   test_in &lt;- read.csv2("test_in.txt",dec=".",sep="\t",header=TRUE)
+   write.table(test_in[,1],file="test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)
+}
+test_out&lt;-test_in[,1]
+print(getwd())
+gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
+png(filename="testdiagram.png")
 print(gplot)
 dev.off()</t>
   </si>
@@ -590,7 +597,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="testdiagram.png"/>
+        <xdr:cNvPr id="2" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -609,7 +616,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2676525" y="1133475"/>
+          <a:off x="2752725" y="1133475"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -634,8 +641,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>685800</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>1333500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -688,7 +695,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="testdiagram.png"/>
+        <xdr:cNvPr id="4" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -737,7 +744,7 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="testdiagram.png"/>
+        <xdr:cNvPr id="3" name="testdiagram.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1060,12 +1067,12 @@
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4:U5"/>
+      <selection activeCell="B1" sqref="B1:H301"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="11" customWidth="1"/>
     <col min="2" max="8" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" customWidth="1"/>
     <col min="18" max="18" width="12.42578125" customWidth="1"/>
@@ -1160,7 +1167,7 @@
         <v>8</v>
       </c>
       <c r="O2" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>1</v>
@@ -1169,13 +1176,13 @@
         <v>8</v>
       </c>
       <c r="R2" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -1217,7 +1224,7 @@
         <v>9</v>
       </c>
       <c r="O3" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>6</v>
@@ -1226,7 +1233,7 @@
         <v>9</v>
       </c>
       <c r="R3" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>6</v>
@@ -1274,7 +1281,7 @@
         <v>10</v>
       </c>
       <c r="O4" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>5</v>
@@ -1283,7 +1290,7 @@
         <v>10</v>
       </c>
       <c r="R4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>5</v>
@@ -1293,7 +1300,7 @@
       </c>
       <c r="U4" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20190726</v>
+        <v>unterverz/unterunterverz/20190807</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -1335,7 +1342,7 @@
         <v>4</v>
       </c>
       <c r="O5" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>7</v>
@@ -1344,7 +1351,7 @@
         <v>4</v>
       </c>
       <c r="R5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>7</v>
@@ -1354,7 +1361,7 @@
       </c>
       <c r="U5" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20190726</v>
+        <v>unterverz/unterunterverz/20190807</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -1418,7 +1425,7 @@
       <c r="M7" s="7"/>
       <c r="U7" s="22" t="str">
         <f ca="1">"unterverz/unterunterverz/"&amp;TEXT(TODAY(),"JJJJMMTT")</f>
-        <v>unterverz/unterunterverz/20190726</v>
+        <v>unterverz/unterunterverz/20190807</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -2594,13 +2601,13 @@
         <v>1.7000000000000001E-2</v>
       </c>
       <c r="F48" s="25" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G48" s="25" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="H48" s="25" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I48" s="7"/>
     </row>
@@ -2623,10 +2630,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:M302"/>
+  <dimension ref="A1:M298"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2639,7 +2646,7 @@
     <col min="18" max="18" width="86.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B1" s="9" t="s">
         <v>22</v>
       </c>
@@ -2650,7 +2657,7 @@
       <c r="G1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" s="9" t="s">
         <v>23</v>
       </c>
@@ -2661,7 +2668,7 @@
       <c r="G2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>24</v>
       </c>
@@ -2672,7 +2679,7 @@
       <c r="G3"/>
       <c r="H3"/>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B4" s="9" t="s">
         <v>25</v>
       </c>
@@ -2683,9 +2690,9 @@
       <c r="G4"/>
       <c r="H4"/>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2694,9 +2701,9 @@
       <c r="G5"/>
       <c r="H5"/>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>27</v>
+        <v>57</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -2705,9 +2712,9 @@
       <c r="G6"/>
       <c r="H6"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
-        <v>28</v>
+        <v>58</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -2716,9 +2723,10 @@
       <c r="G7"/>
       <c r="H7"/>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
-        <v>29</v>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="9" t="str">
+        <f ca="1">"  write.table(test_in[,1],file="""&amp;variablesVerzeichnis&amp;"/test_out.txt"",sep=""\t"",row.names=FALSE,col.names=FALSE,quote=FALSE)"</f>
+        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20190807/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2727,9 +2735,9 @@
       <c r="G8"/>
       <c r="H8"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9"/>
       <c r="D9"/>
@@ -2738,9 +2746,9 @@
       <c r="G9"/>
       <c r="H9"/>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -2749,9 +2757,10 @@
       <c r="G10"/>
       <c r="H10"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="9" t="s">
-        <v>32</v>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="9" t="str">
+        <f ca="1">"png(filename="""&amp;variablesVerzeichnis&amp;"/testdiagram.png"")"</f>
+        <v>png(filename="unterverz/unterunterverz/20190807/testdiagram.png")</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -2760,9 +2769,9 @@
       <c r="G11"/>
       <c r="H11"/>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -2771,10 +2780,9 @@
       <c r="G12"/>
       <c r="H12"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="9" t="str">
-        <f ca="1">"write.table(test_in[,1],file="""&amp;variablesVerzeichnis&amp;"/test_out.txt"",sep=""\t"",row.names=FALSE,col.names=FALSE,quote=FALSE)"</f>
-        <v>write.table(test_in[,1],file="unterverz/unterunterverz/20190726/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="10" t="s">
+        <v>29</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -2783,10 +2791,9 @@
       <c r="G13"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="s">
-        <v>34</v>
-      </c>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14"/>
+      <c r="B14"/>
       <c r="C14"/>
       <c r="D14"/>
       <c r="E14"/>
@@ -2794,10 +2801,12 @@
       <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="9" t="str">
-        <f ca="1">"png(filename="""&amp;variablesVerzeichnis&amp;"/testdiagram.png"")"</f>
-        <v>png(filename="unterverz/unterunterverz/20190726/testdiagram.png")</v>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
       </c>
       <c r="C15"/>
       <c r="D15"/>
@@ -2806,9 +2815,12 @@
       <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="9" t="s">
-        <v>35</v>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -2818,8 +2830,11 @@
       <c r="H16"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B17" s="10" t="s">
-        <v>36</v>
+      <c r="A17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
       </c>
       <c r="C17"/>
       <c r="D17"/>
@@ -2829,9 +2844,16 @@
       <c r="H17"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18"/>
-      <c r="B18"/>
-      <c r="C18"/>
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="str">
+        <f ca="1">variablesVerzeichnis</f>
+        <v>unterverz/unterunterverz/20190807</v>
+      </c>
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
@@ -2839,13 +2861,16 @@
       <c r="H18"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>2</v>
+      <c r="A19" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19"/>
+        <v>30</v>
+      </c>
+      <c r="C19" t="str">
+        <f ca="1">variablesVerzeichnis</f>
+        <v>unterverz/unterunterverz/20190807</v>
+      </c>
       <c r="D19"/>
       <c r="E19"/>
       <c r="F19"/>
@@ -2853,12 +2878,8 @@
       <c r="H19"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>48</v>
-      </c>
+      <c r="A20"/>
+      <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
@@ -2867,11 +2888,11 @@
       <c r="H20"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
+      <c r="A21" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B21" s="13" t="s">
+        <v>3</v>
       </c>
       <c r="C21"/>
       <c r="D21"/>
@@ -2880,43 +2901,40 @@
       <c r="G21"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" t="str">
-        <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20190726</v>
-      </c>
-      <c r="D22"/>
+    <row r="22" spans="1:8" ht="191.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22"/>
       <c r="E22"/>
       <c r="F22"/>
       <c r="G22"/>
       <c r="H22"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" t="str">
-        <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20190726</v>
-      </c>
-      <c r="D23"/>
+      <c r="A23" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23"/>
+      <c r="D23" s="23"/>
       <c r="E23"/>
       <c r="F23"/>
       <c r="G23"/>
       <c r="H23"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24"/>
-      <c r="B24"/>
+      <c r="A24" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>10</v>
+      </c>
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
@@ -2925,11 +2943,11 @@
       <c r="H24"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>3</v>
+      <c r="A25" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>4</v>
       </c>
       <c r="C25"/>
       <c r="D25"/>
@@ -2938,40 +2956,31 @@
       <c r="G25"/>
       <c r="H25"/>
     </row>
-    <row r="26" spans="1:8" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B26" s="15" t="s">
-        <v>37</v>
+    <row r="26" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A26"/>
+      <c r="B26" s="24" t="s">
+        <v>51</v>
       </c>
       <c r="C26"/>
+      <c r="D26"/>
       <c r="E26"/>
       <c r="F26"/>
       <c r="G26"/>
       <c r="H26"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>9</v>
-      </c>
+      <c r="A27"/>
+      <c r="B27"/>
       <c r="C27"/>
-      <c r="D27" s="23"/>
+      <c r="D27"/>
       <c r="E27"/>
       <c r="F27"/>
       <c r="G27"/>
       <c r="H27"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>10</v>
-      </c>
+      <c r="A28"/>
+      <c r="B28"/>
       <c r="C28"/>
       <c r="D28"/>
       <c r="E28"/>
@@ -2980,12 +2989,8 @@
       <c r="H28"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>4</v>
-      </c>
+      <c r="A29"/>
+      <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
       <c r="E29"/>
@@ -2993,11 +2998,9 @@
       <c r="G29"/>
       <c r="H29"/>
     </row>
-    <row r="30" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30"/>
-      <c r="B30" s="24" t="s">
-        <v>59</v>
-      </c>
+      <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
       <c r="E30"/>
@@ -3126,44 +3129,108 @@
       <c r="H42"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A43"/>
-      <c r="B43"/>
-      <c r="C43"/>
-      <c r="D43"/>
-      <c r="E43"/>
-      <c r="F43"/>
-      <c r="G43"/>
-      <c r="H43"/>
+      <c r="B43" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G43" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A44"/>
-      <c r="B44"/>
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
-      <c r="F44"/>
-      <c r="G44"/>
-      <c r="H44"/>
+      <c r="B44" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C44" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J44" s="7"/>
+      <c r="L44" s="7"/>
+      <c r="M44" s="7"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A45"/>
-      <c r="B45"/>
-      <c r="C45"/>
-      <c r="D45"/>
-      <c r="E45"/>
-      <c r="F45"/>
-      <c r="G45"/>
-      <c r="H45"/>
+      <c r="B45" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C45" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G45" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="7"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46"/>
-      <c r="B46"/>
-      <c r="C46"/>
-      <c r="D46"/>
-      <c r="E46"/>
-      <c r="F46"/>
-      <c r="G46"/>
-      <c r="H46"/>
+      <c r="B46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J46" s="7"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="7"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B47" s="11" t="s">
@@ -3292,8 +3359,6 @@
         <v>0</v>
       </c>
       <c r="J51" s="7"/>
-      <c r="L51" s="7"/>
-      <c r="M51" s="7"/>
     </row>
     <row r="52" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B52" s="11" t="s">
@@ -3317,9 +3382,6 @@
       <c r="H52" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J52" s="7"/>
-      <c r="L52" s="7"/>
-      <c r="M52" s="7"/>
     </row>
     <row r="53" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B53" s="11" t="s">
@@ -3343,9 +3405,6 @@
       <c r="H53" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J53" s="7"/>
-      <c r="L53" s="7"/>
-      <c r="M53" s="7"/>
     </row>
     <row r="54" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B54" s="11" t="s">
@@ -3369,9 +3428,6 @@
       <c r="H54" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J54" s="7"/>
-      <c r="L54" s="7"/>
-      <c r="M54" s="7"/>
     </row>
     <row r="55" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B55" s="11" t="s">
@@ -3395,7 +3451,6 @@
       <c r="H55" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="J55" s="7"/>
     </row>
     <row r="56" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B56" s="11" t="s">
@@ -8983,98 +9038,6 @@
         <v>0</v>
       </c>
       <c r="H298" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="299" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B299" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C299" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D299" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E299" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F299" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G299" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H299" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="300" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B300" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C300" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D300" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E300" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F300" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G300" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H300" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="301" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B301" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C301" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D301" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E301" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F301" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G301" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H301" s="11" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="302" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B302" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C302" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D302" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E302" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F302" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G302" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="H302" s="11" t="s">
         <v>0</v>
       </c>
     </row>
@@ -9094,7 +9057,7 @@
   <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I53" sqref="I53"/>
+      <selection activeCell="J7" sqref="J7:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9204,7 +9167,7 @@
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -9237,7 +9200,7 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -9246,7 +9209,7 @@
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -9258,10 +9221,10 @@
         <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -9289,7 +9252,7 @@
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -9298,7 +9261,7 @@
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -9307,7 +9270,7 @@
         <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -9429,10 +9392,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9445,10 +9408,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>20</v>
@@ -9477,10 +9440,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D2">
         <v>42736</v>
@@ -9498,7 +9461,7 @@
         <v>0.1</v>
       </c>
       <c r="I2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J2" s="1">
         <v>3</v>
@@ -9512,7 +9475,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="D3">
         <v>42737</v>
@@ -9530,7 +9493,7 @@
         <v>0.8</v>
       </c>
       <c r="I3" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="J3" s="1">
         <v>3</v>
@@ -9544,7 +9507,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D4">
         <v>42738</v>
@@ -9562,7 +9525,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J4" s="1">
         <v>3</v>
@@ -9576,7 +9539,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -9604,7 +9567,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -9619,7 +9582,7 @@
         <v>0.1</v>
       </c>
       <c r="J9" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -9630,7 +9593,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="F10">
         <v>68.56</v>
@@ -9645,7 +9608,7 @@
         <v>0.8</v>
       </c>
       <c r="J10" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="K10" s="22">
         <v>3</v>
@@ -9656,7 +9619,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="F11">
         <v>300</v>
@@ -9671,7 +9634,7 @@
         <v>5</v>
       </c>
       <c r="J11" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="K11" s="22">
         <v>3</v>
@@ -9685,18 +9648,26 @@
     </row>
     <row r="39" spans="1:2" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>39</v>
+      <c r="B41" s="19" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed closing bug (not removing menu items)
</commit_message>
<xml_diff>
--- a/test/testRAddin.xlsx
+++ b/test/testRAddin.xlsx
@@ -1300,7 +1300,7 @@
       </c>
       <c r="U4" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20190807</v>
+        <v>unterverz/unterunterverz/20200210</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -1361,7 +1361,7 @@
       </c>
       <c r="U5" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20190807</v>
+        <v>unterverz/unterunterverz/20200210</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -1425,7 +1425,7 @@
       <c r="M7" s="7"/>
       <c r="U7" s="22" t="str">
         <f ca="1">"unterverz/unterunterverz/"&amp;TEXT(TODAY(),"JJJJMMTT")</f>
-        <v>unterverz/unterunterverz/20190807</v>
+        <v>unterverz/unterunterverz/20200210</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -2633,7 +2633,7 @@
   <dimension ref="A1:M298"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2726,7 +2726,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="str">
         <f ca="1">"  write.table(test_in[,1],file="""&amp;variablesVerzeichnis&amp;"/test_out.txt"",sep=""\t"",row.names=FALSE,col.names=FALSE,quote=FALSE)"</f>
-        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20190807/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
+        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20200210/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2760,7 +2760,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="str">
         <f ca="1">"png(filename="""&amp;variablesVerzeichnis&amp;"/testdiagram.png"")"</f>
-        <v>png(filename="unterverz/unterunterverz/20190807/testdiagram.png")</v>
+        <v>png(filename="unterverz/unterunterverz/20200210/testdiagram.png")</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -2852,7 +2852,7 @@
       </c>
       <c r="C18" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20190807</v>
+        <v>unterverz/unterunterverz/20200210</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="C19" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20190807</v>
+        <v>unterverz/unterunterverz/20200210</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>

</xml_diff>

<commit_message>
added Distribution changed script execution from shell to process
</commit_message>
<xml_diff>
--- a/test/testRAddin.xlsx
+++ b/test/testRAddin.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\RAddin\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA0AFC1-6F4B-4EFA-8B59-C610759C3409}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1470" windowWidth="18795" windowHeight="7830" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -19,6 +25,8 @@
     <definedName name="Data_3" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
     <definedName name="Data_4" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
     <definedName name="Data_5" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
+    <definedName name="Data_6" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
+    <definedName name="Data_7" localSheetId="0">'Main Test'!$A$2:$A$48</definedName>
     <definedName name="R_Addin" localSheetId="2">Test_OtherSheet!$J$1:$L$5</definedName>
     <definedName name="R_Addin" localSheetId="3">Test_RdotNet!$A$1:$C$5</definedName>
     <definedName name="R_Addin">'Main Test'!$J$1:$L$5</definedName>
@@ -43,12 +51,15 @@
     <definedName name="testdiagram">'Main Test'!$J$8</definedName>
     <definedName name="variablesVerzeichnis">'Main Test'!$U$7</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -56,85 +67,85 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="test_out" type="6" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="test_out" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="test_out1" type="6" refreshedVersion="0" background="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="test_out1" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="test_out10" type="6" refreshedVersion="0" background="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="test_out10" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="test_out2" type="6" refreshedVersion="0" background="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="test_out2" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" name="test_out21" type="6" refreshedVersion="0" background="1">
+  <connection id="5" xr16:uid="{00000000-0015-0000-FFFF-FFFF04000000}" name="test_out21" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\\test_out2.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" name="test_out3" type="6" refreshedVersion="0" background="1">
+  <connection id="6" xr16:uid="{00000000-0015-0000-FFFF-FFFF05000000}" name="test_out3" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="7" name="test_out4" type="6" refreshedVersion="0" background="1">
+  <connection id="7" xr16:uid="{00000000-0015-0000-FFFF-FFFF06000000}" name="test_out4" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="8" name="test_out5" type="6" refreshedVersion="0" background="1">
+  <connection id="8" xr16:uid="{00000000-0015-0000-FFFF-FFFF07000000}" name="test_out5" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\testDirNonExisting\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="9" name="test_out6" type="6" refreshedVersion="0" background="1">
+  <connection id="9" xr16:uid="{00000000-0015-0000-FFFF-FFFF08000000}" name="test_out6" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="10" name="test_out7" type="6" refreshedVersion="0" background="1">
+  <connection id="10" xr16:uid="{00000000-0015-0000-FFFF-FFFF09000000}" name="test_out7" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="11" name="test_out8" type="6" refreshedVersion="0" background="1">
+  <connection id="11" xr16:uid="{00000000-0015-0000-FFFF-FFFF0A000000}" name="test_out8" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
-  <connection id="12" name="test_out9" type="6" refreshedVersion="0" background="1">
+  <connection id="12" xr16:uid="{00000000-0015-0000-FFFF-FFFF0B000000}" name="test_out9" type="6" refreshedVersion="0" background="1">
     <textPr prompt="0" sourceFile="C:\dev\RAddin\trunk\test\.\test_out.txt" decimal="," thousands=".">
       <textFields>
         <textField/>
@@ -145,7 +156,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1950" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1947" uniqueCount="57">
   <si>
     <t/>
   </si>
@@ -228,9 +239,6 @@
     <t>}</t>
   </si>
   <si>
-    <t>gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()</t>
-  </si>
-  <si>
     <t>print(gplot)</t>
   </si>
   <si>
@@ -291,15 +299,6 @@
     <t>ret</t>
   </si>
   <si>
-    <t>ä</t>
-  </si>
-  <si>
-    <t>ö</t>
-  </si>
-  <si>
-    <t>ß</t>
-  </si>
-  <si>
     <t>-&gt; Attention, diagram for test_scriptcell appears in Main Test !!!</t>
   </si>
   <si>
@@ -348,16 +347,19 @@
 }
 test_out&lt;-test_in[,1]
 print(getwd())
-gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
+gplot &lt;- ggplot(data = test_in, aes(x = in3, y = in4) ) + geom_point()
 png(filename="testdiagram.png")
 print(gplot)
 dev.off()</t>
+  </si>
+  <si>
+    <t>gplot &lt;- ggplot(data = test_in, aes(x = in5, y = in6) ) + geom_point()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="\."/>
@@ -524,15 +526,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Komma 2" xfId="3"/>
-    <cellStyle name="Prozent 2" xfId="4"/>
+    <cellStyle name="Komma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Prozent 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
-    <cellStyle name="Standard 2 2" xfId="5"/>
-    <cellStyle name="Standard 3" xfId="2"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Standard 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Standard 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -559,7 +561,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -597,7 +599,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="testdiagram.png"/>
+        <xdr:cNvPr id="3" name="testdiagram.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90E4BB58-1732-4B0B-8BB2-7B8801105CEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -616,7 +624,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2752725" y="1133475"/>
+          <a:off x="2828925" y="1133475"/>
           <a:ext cx="4572000" cy="4572000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -646,7 +654,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="testdiagram.png"/>
+        <xdr:cNvPr id="4" name="testdiagram.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{741ECA18-5151-42F1-AB02-52E961ECE795}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -695,7 +709,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="testdiagram.png"/>
+        <xdr:cNvPr id="5" name="testdiagram.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{340D5524-85F5-4956-A1BE-1A269D2F52C2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -727,59 +747,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>3810000</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="testdiagram.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="2409825"/>
-          <a:ext cx="4572000" cy="4572000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -817,9 +788,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -852,9 +823,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -887,9 +875,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1062,18 +1067,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="eingabe"/>
   <dimension ref="A1:U50"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H301"/>
+      <selection activeCell="M1" sqref="M1:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.7109375" style="11" customWidth="1"/>
-    <col min="2" max="8" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="4.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.140625" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5703125" customWidth="1"/>
     <col min="18" max="18" width="12.42578125" customWidth="1"/>
   </cols>
@@ -1111,21 +1119,21 @@
       </c>
       <c r="N1" t="str">
         <f ca="1">SUBSTITUTE(CELL("DATEINAME",O1),"[testRAddin.xlsx]Main Test","")</f>
-        <v>C:\dev\RAddin\trunk\test\</v>
+        <v>C:\dev\RAddin\test\</v>
       </c>
       <c r="P1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="Q1" t="str">
         <f ca="1">SUBSTITUTE(CELL("DATEINAME",R1),"[testRAddin.xlsx]Main Test","")</f>
-        <v>C:\dev\RAddin\trunk\test\</v>
+        <v>C:\dev\RAddin\test\</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="T1" t="str">
         <f ca="1">SUBSTITUTE(CELL("DATEINAME",U1),"[testRAddin.xlsx]Main Test","")</f>
-        <v>C:\dev\RAddin\trunk\test\</v>
+        <v>C:\dev\RAddin\test\</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -1139,19 +1147,19 @@
         <v>0.40250000000000002</v>
       </c>
       <c r="D2" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="E2" s="11">
-        <v>0.29749999999999999</v>
+        <v>-0.29749999999999993</v>
       </c>
       <c r="F2" s="11">
-        <v>0.40250000000000002</v>
+        <v>0.99749999999999983</v>
       </c>
       <c r="G2" s="11">
-        <v>0.29749999999999999</v>
+        <v>1.2949999999999997</v>
       </c>
       <c r="H2" s="11">
-        <v>0.40250000000000002</v>
+        <v>-1.8899999999999995</v>
       </c>
       <c r="I2" s="7"/>
       <c r="J2" s="3" t="s">
@@ -1167,7 +1175,7 @@
         <v>8</v>
       </c>
       <c r="O2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>1</v>
@@ -1176,13 +1184,13 @@
         <v>8</v>
       </c>
       <c r="R2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -1196,19 +1204,19 @@
         <v>0.50719999999999998</v>
       </c>
       <c r="D3" s="11">
-        <v>0.30690000000000001</v>
+        <v>0.81410000000000005</v>
       </c>
       <c r="E3" s="11">
-        <v>0.30690000000000001</v>
+        <v>-0.30690000000000006</v>
       </c>
       <c r="F3" s="11">
-        <v>0.50719999999999998</v>
+        <v>1.121</v>
       </c>
       <c r="G3" s="11">
-        <v>0.30690000000000001</v>
+        <v>1.4279000000000002</v>
       </c>
       <c r="H3" s="11">
-        <v>0.50719999999999998</v>
+        <v>-2.0417000000000001</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="3" t="s">
@@ -1224,7 +1232,7 @@
         <v>9</v>
       </c>
       <c r="O3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>6</v>
@@ -1233,7 +1241,7 @@
         <v>9</v>
       </c>
       <c r="R3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>6</v>
@@ -1253,19 +1261,19 @@
         <v>1.7100000000000001E-2</v>
       </c>
       <c r="D4" s="11">
-        <v>1.04E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="E4" s="11">
-        <v>1.04E-2</v>
+        <v>-1.04E-2</v>
       </c>
       <c r="F4" s="11">
-        <v>1.7100000000000001E-2</v>
+        <v>3.7900000000000003E-2</v>
       </c>
       <c r="G4" s="11">
-        <v>1.04E-2</v>
+        <v>4.8299999999999996E-2</v>
       </c>
       <c r="H4" s="11">
-        <v>1.7100000000000001E-2</v>
+        <v>-6.9099999999999995E-2</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="3" t="s">
@@ -1281,7 +1289,7 @@
         <v>10</v>
       </c>
       <c r="O4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>5</v>
@@ -1290,7 +1298,7 @@
         <v>10</v>
       </c>
       <c r="R4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>5</v>
@@ -1300,7 +1308,7 @@
       </c>
       <c r="U4" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20200210</v>
+        <v>unterverz/unterunterverz/20210306</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -1314,19 +1322,19 @@
         <v>6.8999999999999999E-3</v>
       </c>
       <c r="D5" s="11">
-        <v>5.1000000000000004E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="E5" s="11">
-        <v>5.1000000000000004E-3</v>
+        <v>-5.1000000000000004E-3</v>
       </c>
       <c r="F5" s="11">
-        <v>6.8999999999999999E-3</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="G5" s="11">
-        <v>5.1000000000000004E-3</v>
+        <v>2.2200000000000001E-2</v>
       </c>
       <c r="H5" s="11">
-        <v>6.8999999999999999E-3</v>
+        <v>-3.2399999999999998E-2</v>
       </c>
       <c r="I5" s="7"/>
       <c r="J5" s="3" t="s">
@@ -1342,7 +1350,7 @@
         <v>4</v>
       </c>
       <c r="O5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>7</v>
@@ -1351,7 +1359,7 @@
         <v>4</v>
       </c>
       <c r="R5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>7</v>
@@ -1361,7 +1369,7 @@
       </c>
       <c r="U5" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20200210</v>
+        <v>unterverz/unterunterverz/20210306</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -1375,19 +1383,19 @@
         <v>0.28749999999999998</v>
       </c>
       <c r="D6" s="11">
-        <v>0.21249999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="E6" s="11">
-        <v>0.21249999999999999</v>
+        <v>-0.21250000000000002</v>
       </c>
       <c r="F6" s="11">
-        <v>0.28749999999999998</v>
+        <v>0.71250000000000002</v>
       </c>
       <c r="G6" s="11">
-        <v>0.21249999999999999</v>
+        <v>0.92499999999999993</v>
       </c>
       <c r="H6" s="11">
-        <v>0.28749999999999998</v>
+        <v>-1.35</v>
       </c>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
@@ -1405,19 +1413,19 @@
         <v>8.8999999999999999E-3</v>
       </c>
       <c r="D7" s="11">
-        <v>5.4999999999999997E-3</v>
+        <v>1.44E-2</v>
       </c>
       <c r="E7" s="11">
-        <v>5.4999999999999997E-3</v>
+        <v>-5.4999999999999997E-3</v>
       </c>
       <c r="F7" s="11">
-        <v>8.8999999999999999E-3</v>
+        <v>1.9900000000000001E-2</v>
       </c>
       <c r="G7" s="11">
-        <v>5.4999999999999997E-3</v>
+        <v>2.5399999999999999E-2</v>
       </c>
       <c r="H7" s="11">
-        <v>8.8999999999999999E-3</v>
+        <v>-3.6400000000000002E-2</v>
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
@@ -1425,7 +1433,7 @@
       <c r="M7" s="7"/>
       <c r="U7" s="22" t="str">
         <f ca="1">"unterverz/unterunterverz/"&amp;TEXT(TODAY(),"JJJJMMTT")</f>
-        <v>unterverz/unterunterverz/20200210</v>
+        <v>unterverz/unterunterverz/20210306</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -1439,19 +1447,19 @@
         <v>1.15E-2</v>
       </c>
       <c r="D8" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>0.02</v>
       </c>
       <c r="E8" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>-8.5000000000000006E-3</v>
       </c>
       <c r="F8" s="11">
-        <v>1.15E-2</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="G8" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="H8" s="11">
-        <v>1.15E-2</v>
+        <v>-5.4000000000000006E-2</v>
       </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
@@ -1469,19 +1477,19 @@
         <v>1.61E-2</v>
       </c>
       <c r="D9" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="E9" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>-1.1900000000000001E-2</v>
       </c>
       <c r="F9" s="11">
-        <v>1.61E-2</v>
+        <v>3.9900000000000005E-2</v>
       </c>
       <c r="G9" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="H9" s="11">
-        <v>1.61E-2</v>
+        <v>-7.5600000000000001E-2</v>
       </c>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
@@ -1499,19 +1507,19 @@
         <v>3.1099999999999999E-2</v>
       </c>
       <c r="D10" s="11">
-        <v>2.3E-2</v>
+        <v>5.4099999999999995E-2</v>
       </c>
       <c r="E10" s="11">
-        <v>2.3E-2</v>
+        <v>-2.2999999999999996E-2</v>
       </c>
       <c r="F10" s="11">
-        <v>3.1099999999999999E-2</v>
+        <v>7.7099999999999988E-2</v>
       </c>
       <c r="G10" s="11">
-        <v>2.3E-2</v>
+        <v>0.10009999999999998</v>
       </c>
       <c r="H10" s="11">
-        <v>3.1099999999999999E-2</v>
+        <v>-0.14609999999999998</v>
       </c>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
@@ -1529,19 +1537,19 @@
         <v>0.63400000000000001</v>
       </c>
       <c r="D11" s="11">
-        <v>0.3836</v>
+        <v>1.0176000000000001</v>
       </c>
       <c r="E11" s="11">
-        <v>0.3836</v>
+        <v>-0.38360000000000005</v>
       </c>
       <c r="F11" s="11">
-        <v>0.63400000000000001</v>
+        <v>1.4012000000000002</v>
       </c>
       <c r="G11" s="11">
-        <v>0.3836</v>
+        <v>1.7848000000000002</v>
       </c>
       <c r="H11" s="11">
-        <v>0.63400000000000001</v>
+        <v>-2.552</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -1559,19 +1567,19 @@
         <v>0.5706</v>
       </c>
       <c r="D12" s="11">
-        <v>0.34520000000000001</v>
+        <v>0.91579999999999995</v>
       </c>
       <c r="E12" s="11">
-        <v>0.34520000000000001</v>
+        <v>-0.34519999999999995</v>
       </c>
       <c r="F12" s="11">
-        <v>0.5706</v>
+        <v>1.2609999999999999</v>
       </c>
       <c r="G12" s="11">
-        <v>0.34520000000000001</v>
+        <v>1.6062000000000001</v>
       </c>
       <c r="H12" s="11">
-        <v>0.5706</v>
+        <v>-2.2965999999999998</v>
       </c>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
@@ -1589,19 +1597,19 @@
         <v>2.4E-2</v>
       </c>
       <c r="D13" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>3.85E-2</v>
       </c>
       <c r="E13" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>-1.4499999999999999E-2</v>
       </c>
       <c r="F13" s="11">
-        <v>2.4E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="G13" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="H13" s="11">
-        <v>2.4E-2</v>
+        <v>-9.6500000000000002E-2</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
@@ -1619,19 +1627,19 @@
         <v>2.4E-2</v>
       </c>
       <c r="D14" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>3.85E-2</v>
       </c>
       <c r="E14" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>-1.4499999999999999E-2</v>
       </c>
       <c r="F14" s="11">
-        <v>2.4E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="G14" s="11">
-        <v>1.4500000000000001E-2</v>
+        <v>6.7500000000000004E-2</v>
       </c>
       <c r="H14" s="11">
-        <v>2.4E-2</v>
+        <v>-9.6500000000000002E-2</v>
       </c>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
@@ -1649,19 +1657,19 @@
         <v>1.38E-2</v>
       </c>
       <c r="D15" s="11">
-        <v>1.0200000000000001E-2</v>
+        <v>2.4E-2</v>
       </c>
       <c r="E15" s="11">
-        <v>1.0200000000000001E-2</v>
+        <v>-1.0200000000000001E-2</v>
       </c>
       <c r="F15" s="11">
-        <v>1.38E-2</v>
+        <v>3.4200000000000001E-2</v>
       </c>
       <c r="G15" s="11">
-        <v>1.0200000000000001E-2</v>
+        <v>4.4400000000000002E-2</v>
       </c>
       <c r="H15" s="11">
-        <v>1.38E-2</v>
+        <v>-6.4799999999999996E-2</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -1679,19 +1687,19 @@
         <v>0.40250000000000002</v>
       </c>
       <c r="D16" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="E16" s="11">
-        <v>0.29749999999999999</v>
+        <v>-0.29749999999999993</v>
       </c>
       <c r="F16" s="11">
-        <v>0.40250000000000002</v>
+        <v>0.99749999999999983</v>
       </c>
       <c r="G16" s="11">
-        <v>0.29749999999999999</v>
+        <v>1.2949999999999997</v>
       </c>
       <c r="H16" s="11">
-        <v>0.40250000000000002</v>
+        <v>-1.8899999999999995</v>
       </c>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -1709,19 +1717,19 @@
         <v>0.40250000000000002</v>
       </c>
       <c r="D17" s="11">
-        <v>0.29749999999999999</v>
+        <v>0.7</v>
       </c>
       <c r="E17" s="11">
-        <v>0.29749999999999999</v>
+        <v>-0.29749999999999993</v>
       </c>
       <c r="F17" s="11">
-        <v>0.40250000000000002</v>
+        <v>0.99749999999999983</v>
       </c>
       <c r="G17" s="11">
-        <v>0.29749999999999999</v>
+        <v>1.2949999999999997</v>
       </c>
       <c r="H17" s="11">
-        <v>0.40250000000000002</v>
+        <v>-1.8899999999999995</v>
       </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
@@ -1739,19 +1747,19 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="D18" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="E18" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>-7.700000000000002E-3</v>
       </c>
       <c r="F18" s="11">
-        <v>1.2699999999999999E-2</v>
+        <v>2.8100000000000003E-2</v>
       </c>
       <c r="G18" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>3.5799999999999998E-2</v>
       </c>
       <c r="H18" s="11">
-        <v>1.2699999999999999E-2</v>
+        <v>-5.1199999999999996E-2</v>
       </c>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -1769,19 +1777,19 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="D19" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="E19" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>-7.700000000000002E-3</v>
       </c>
       <c r="F19" s="11">
-        <v>1.2699999999999999E-2</v>
+        <v>2.8100000000000003E-2</v>
       </c>
       <c r="G19" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>3.5799999999999998E-2</v>
       </c>
       <c r="H19" s="11">
-        <v>1.2699999999999999E-2</v>
+        <v>-5.1199999999999996E-2</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -1799,19 +1807,19 @@
         <v>1.61E-2</v>
       </c>
       <c r="D20" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="E20" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>-1.1900000000000001E-2</v>
       </c>
       <c r="F20" s="11">
-        <v>1.61E-2</v>
+        <v>3.9900000000000005E-2</v>
       </c>
       <c r="G20" s="11">
-        <v>1.1900000000000001E-2</v>
+        <v>5.1799999999999999E-2</v>
       </c>
       <c r="H20" s="11">
-        <v>1.61E-2</v>
+        <v>-7.5600000000000001E-2</v>
       </c>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -1829,19 +1837,19 @@
         <v>2.3E-2</v>
       </c>
       <c r="D21" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E21" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>-1.7000000000000001E-2</v>
       </c>
       <c r="F21" s="11">
-        <v>2.3E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="G21" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>7.400000000000001E-2</v>
       </c>
       <c r="H21" s="11">
-        <v>2.3E-2</v>
+        <v>-0.10800000000000001</v>
       </c>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
@@ -1859,19 +1867,19 @@
         <v>2.5899999999999999E-2</v>
       </c>
       <c r="D22" s="11">
-        <v>1.9099999999999999E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="E22" s="11">
-        <v>1.9099999999999999E-2</v>
+        <v>-1.9099999999999999E-2</v>
       </c>
       <c r="F22" s="11">
-        <v>2.5899999999999999E-2</v>
+        <v>6.409999999999999E-2</v>
       </c>
       <c r="G22" s="11">
-        <v>1.9099999999999999E-2</v>
+        <v>8.3199999999999996E-2</v>
       </c>
       <c r="H22" s="11">
-        <v>2.5899999999999999E-2</v>
+        <v>-0.12139999999999998</v>
       </c>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -1889,19 +1897,19 @@
         <v>5.7500000000000002E-2</v>
       </c>
       <c r="D23" s="11">
-        <v>4.2500000000000003E-2</v>
+        <v>0.1</v>
       </c>
       <c r="E23" s="11">
-        <v>4.2500000000000003E-2</v>
+        <v>-4.2500000000000003E-2</v>
       </c>
       <c r="F23" s="11">
-        <v>5.7500000000000002E-2</v>
+        <v>0.14250000000000002</v>
       </c>
       <c r="G23" s="11">
-        <v>4.2500000000000003E-2</v>
+        <v>0.18500000000000003</v>
       </c>
       <c r="H23" s="11">
-        <v>5.7500000000000002E-2</v>
+        <v>-0.27</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
@@ -1919,19 +1927,19 @@
         <v>5.1799999999999999E-2</v>
       </c>
       <c r="D24" s="11">
-        <v>3.8300000000000001E-2</v>
+        <v>9.01E-2</v>
       </c>
       <c r="E24" s="11">
-        <v>3.8300000000000001E-2</v>
+        <v>-3.8300000000000001E-2</v>
       </c>
       <c r="F24" s="11">
-        <v>5.1799999999999999E-2</v>
+        <v>0.12840000000000001</v>
       </c>
       <c r="G24" s="11">
-        <v>3.8300000000000001E-2</v>
+        <v>0.16670000000000001</v>
       </c>
       <c r="H24" s="11">
-        <v>5.1799999999999999E-2</v>
+        <v>-0.24330000000000002</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
@@ -1949,19 +1957,19 @@
         <v>0.73540000000000005</v>
       </c>
       <c r="D25" s="11">
-        <v>0.44500000000000001</v>
+        <v>1.1804000000000001</v>
       </c>
       <c r="E25" s="11">
-        <v>0.44500000000000001</v>
+        <v>-0.44500000000000006</v>
       </c>
       <c r="F25" s="11">
-        <v>0.73540000000000005</v>
+        <v>1.6254000000000002</v>
       </c>
       <c r="G25" s="11">
-        <v>0.44500000000000001</v>
+        <v>2.0704000000000002</v>
       </c>
       <c r="H25" s="11">
-        <v>0.73540000000000005</v>
+        <v>-2.9604000000000008</v>
       </c>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
@@ -1979,19 +1987,19 @@
         <v>0.54520000000000002</v>
       </c>
       <c r="D26" s="11">
-        <v>0.32979999999999998</v>
+        <v>0.875</v>
       </c>
       <c r="E26" s="11">
-        <v>0.32979999999999998</v>
+        <v>-0.32979999999999998</v>
       </c>
       <c r="F26" s="11">
-        <v>0.54520000000000002</v>
+        <v>1.2048000000000001</v>
       </c>
       <c r="G26" s="11">
-        <v>0.32979999999999998</v>
+        <v>1.5346000000000002</v>
       </c>
       <c r="H26" s="11">
-        <v>0.54520000000000002</v>
+        <v>-2.1942000000000004</v>
       </c>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
@@ -2009,19 +2017,19 @@
         <v>0.59589999999999999</v>
       </c>
       <c r="D27" s="11">
-        <v>0.36049999999999999</v>
+        <v>0.95639999999999992</v>
       </c>
       <c r="E27" s="11">
-        <v>0.36049999999999999</v>
+        <v>-0.36049999999999993</v>
       </c>
       <c r="F27" s="11">
-        <v>0.59589999999999999</v>
+        <v>1.3169</v>
       </c>
       <c r="G27" s="11">
-        <v>0.36049999999999999</v>
+        <v>1.6774</v>
       </c>
       <c r="H27" s="11">
-        <v>0.59589999999999999</v>
+        <v>-2.3984000000000001</v>
       </c>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
@@ -2039,19 +2047,19 @@
         <v>0.317</v>
       </c>
       <c r="D28" s="11">
-        <v>0.1918</v>
+        <v>0.50880000000000003</v>
       </c>
       <c r="E28" s="11">
-        <v>0.1918</v>
+        <v>-0.19180000000000003</v>
       </c>
       <c r="F28" s="11">
-        <v>0.317</v>
+        <v>0.70060000000000011</v>
       </c>
       <c r="G28" s="11">
-        <v>0.1918</v>
+        <v>0.89240000000000008</v>
       </c>
       <c r="H28" s="11">
-        <v>0.317</v>
+        <v>-1.276</v>
       </c>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
@@ -2069,19 +2077,19 @@
         <v>3.0499999999999999E-2</v>
       </c>
       <c r="D29" s="11">
-        <v>1.84E-2</v>
+        <v>4.8899999999999999E-2</v>
       </c>
       <c r="E29" s="11">
-        <v>1.84E-2</v>
+        <v>-1.84E-2</v>
       </c>
       <c r="F29" s="11">
-        <v>3.0499999999999999E-2</v>
+        <v>6.7299999999999999E-2</v>
       </c>
       <c r="G29" s="11">
-        <v>1.84E-2</v>
+        <v>8.5699999999999998E-2</v>
       </c>
       <c r="H29" s="11">
-        <v>3.0499999999999999E-2</v>
+        <v>-0.1225</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
@@ -2099,19 +2107,19 @@
         <v>2.0899999999999998E-2</v>
       </c>
       <c r="D30" s="11">
-        <v>1.26E-2</v>
+        <v>3.3500000000000002E-2</v>
       </c>
       <c r="E30" s="11">
-        <v>1.26E-2</v>
+        <v>-1.2600000000000004E-2</v>
       </c>
       <c r="F30" s="11">
-        <v>2.0899999999999998E-2</v>
+        <v>4.6100000000000002E-2</v>
       </c>
       <c r="G30" s="11">
-        <v>1.26E-2</v>
+        <v>5.8700000000000002E-2</v>
       </c>
       <c r="H30" s="11">
-        <v>2.0899999999999998E-2</v>
+        <v>-8.3900000000000002E-2</v>
       </c>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
@@ -2129,19 +2137,19 @@
         <v>2.0899999999999998E-2</v>
       </c>
       <c r="D31" s="11">
-        <v>1.26E-2</v>
+        <v>3.3500000000000002E-2</v>
       </c>
       <c r="E31" s="11">
-        <v>1.26E-2</v>
+        <v>-1.2600000000000004E-2</v>
       </c>
       <c r="F31" s="11">
-        <v>2.0899999999999998E-2</v>
+        <v>4.6100000000000002E-2</v>
       </c>
       <c r="G31" s="11">
-        <v>1.26E-2</v>
+        <v>5.8700000000000002E-2</v>
       </c>
       <c r="H31" s="11">
-        <v>2.0899999999999998E-2</v>
+        <v>-8.3900000000000002E-2</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
@@ -2159,19 +2167,19 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="D32" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>2.0400000000000001E-2</v>
       </c>
       <c r="E32" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>-7.700000000000002E-3</v>
       </c>
       <c r="F32" s="11">
-        <v>1.2699999999999999E-2</v>
+        <v>2.8100000000000003E-2</v>
       </c>
       <c r="G32" s="11">
-        <v>7.7000000000000002E-3</v>
+        <v>3.5799999999999998E-2</v>
       </c>
       <c r="H32" s="11">
-        <v>1.2699999999999999E-2</v>
+        <v>-5.1199999999999996E-2</v>
       </c>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
@@ -2189,19 +2197,19 @@
         <v>0.46</v>
       </c>
       <c r="D33" s="11">
-        <v>0.34</v>
+        <v>0.8</v>
       </c>
       <c r="E33" s="11">
-        <v>0.34</v>
+        <v>-0.34</v>
       </c>
       <c r="F33" s="11">
-        <v>0.46</v>
+        <v>1.1400000000000001</v>
       </c>
       <c r="G33" s="11">
-        <v>0.34</v>
+        <v>1.4800000000000002</v>
       </c>
       <c r="H33" s="11">
-        <v>0.46</v>
+        <v>-2.16</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
@@ -2217,19 +2225,19 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="D34" s="11">
-        <v>0.255</v>
+        <v>0.6</v>
       </c>
       <c r="E34" s="11">
-        <v>0.255</v>
+        <v>-0.255</v>
       </c>
       <c r="F34" s="11">
-        <v>0.34499999999999997</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="G34" s="11">
-        <v>0.255</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="H34" s="11">
-        <v>0.34499999999999997</v>
+        <v>-1.62</v>
       </c>
       <c r="I34" s="7"/>
     </row>
@@ -2244,19 +2252,19 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="D35" s="11">
-        <v>0.255</v>
+        <v>0.6</v>
       </c>
       <c r="E35" s="11">
-        <v>0.255</v>
+        <v>-0.255</v>
       </c>
       <c r="F35" s="11">
-        <v>0.34499999999999997</v>
+        <v>0.85499999999999998</v>
       </c>
       <c r="G35" s="11">
-        <v>0.255</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="H35" s="11">
-        <v>0.34499999999999997</v>
+        <v>-1.62</v>
       </c>
       <c r="I35" s="7"/>
     </row>
@@ -2271,19 +2279,19 @@
         <v>0.115</v>
       </c>
       <c r="D36" s="11">
-        <v>8.5000000000000006E-2</v>
+        <v>0.2</v>
       </c>
       <c r="E36" s="11">
-        <v>8.5000000000000006E-2</v>
+        <v>-8.5000000000000006E-2</v>
       </c>
       <c r="F36" s="11">
-        <v>0.115</v>
+        <v>0.28500000000000003</v>
       </c>
       <c r="G36" s="11">
-        <v>8.5000000000000006E-2</v>
+        <v>0.37000000000000005</v>
       </c>
       <c r="H36" s="11">
-        <v>0.115</v>
+        <v>-0.54</v>
       </c>
       <c r="I36" s="7"/>
     </row>
@@ -2298,19 +2306,19 @@
         <v>1.9E-2</v>
       </c>
       <c r="D37" s="11">
-        <v>1.15E-2</v>
+        <v>3.0499999999999999E-2</v>
       </c>
       <c r="E37" s="11">
-        <v>1.15E-2</v>
+        <v>-1.15E-2</v>
       </c>
       <c r="F37" s="11">
-        <v>1.9E-2</v>
+        <v>4.1999999999999996E-2</v>
       </c>
       <c r="G37" s="11">
-        <v>1.15E-2</v>
+        <v>5.3499999999999992E-2</v>
       </c>
       <c r="H37" s="11">
-        <v>1.9E-2</v>
+        <v>-7.6499999999999985E-2</v>
       </c>
       <c r="I37" s="7"/>
     </row>
@@ -2325,19 +2333,19 @@
         <v>1.0800000000000001E-2</v>
       </c>
       <c r="D38" s="11">
-        <v>6.6E-3</v>
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="E38" s="11">
-        <v>6.6E-3</v>
+        <v>-6.5999999999999982E-3</v>
       </c>
       <c r="F38" s="11">
-        <v>1.0800000000000001E-2</v>
+        <v>2.3999999999999997E-2</v>
       </c>
       <c r="G38" s="11">
-        <v>6.6E-3</v>
+        <v>3.0599999999999992E-2</v>
       </c>
       <c r="H38" s="11">
-        <v>1.0800000000000001E-2</v>
+        <v>-4.3799999999999992E-2</v>
       </c>
       <c r="I38" s="7"/>
     </row>
@@ -2352,19 +2360,19 @@
         <v>1.0800000000000001E-2</v>
       </c>
       <c r="D39" s="11">
-        <v>6.6E-3</v>
+        <v>1.7399999999999999E-2</v>
       </c>
       <c r="E39" s="11">
-        <v>6.6E-3</v>
+        <v>-6.5999999999999982E-3</v>
       </c>
       <c r="F39" s="11">
-        <v>1.0800000000000001E-2</v>
+        <v>2.3999999999999997E-2</v>
       </c>
       <c r="G39" s="11">
-        <v>6.6E-3</v>
+        <v>3.0599999999999992E-2</v>
       </c>
       <c r="H39" s="11">
-        <v>1.0800000000000001E-2</v>
+        <v>-4.3799999999999992E-2</v>
       </c>
       <c r="I39" s="7"/>
     </row>
@@ -2379,19 +2387,19 @@
         <v>4.4000000000000003E-3</v>
       </c>
       <c r="D40" s="11">
-        <v>2.7000000000000001E-3</v>
+        <v>7.1000000000000004E-3</v>
       </c>
       <c r="E40" s="11">
-        <v>2.7000000000000001E-3</v>
+        <v>-2.7000000000000001E-3</v>
       </c>
       <c r="F40" s="11">
-        <v>4.4000000000000003E-3</v>
+        <v>9.7999999999999997E-3</v>
       </c>
       <c r="G40" s="11">
-        <v>2.7000000000000001E-3</v>
+        <v>1.2499999999999997E-2</v>
       </c>
       <c r="H40" s="11">
-        <v>4.4000000000000003E-3</v>
+        <v>-1.7899999999999996E-2</v>
       </c>
       <c r="I40" s="7"/>
     </row>
@@ -2406,19 +2414,19 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="D41" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E41" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>-3.4000000000000002E-2</v>
       </c>
       <c r="F41" s="11">
-        <v>4.5999999999999999E-2</v>
+        <v>0.114</v>
       </c>
       <c r="G41" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>0.14800000000000002</v>
       </c>
       <c r="H41" s="11">
-        <v>4.5999999999999999E-2</v>
+        <v>-0.21600000000000003</v>
       </c>
       <c r="I41" s="7"/>
     </row>
@@ -2433,19 +2441,19 @@
         <v>2.3E-2</v>
       </c>
       <c r="D42" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E42" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>-1.7000000000000001E-2</v>
       </c>
       <c r="F42" s="11">
-        <v>2.3E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="G42" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>7.400000000000001E-2</v>
       </c>
       <c r="H42" s="11">
-        <v>2.3E-2</v>
+        <v>-0.10800000000000001</v>
       </c>
       <c r="I42" s="7"/>
     </row>
@@ -2460,19 +2468,19 @@
         <v>2.01E-2</v>
       </c>
       <c r="D43" s="11">
-        <v>1.49E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="E43" s="11">
-        <v>1.49E-2</v>
+        <v>-1.4900000000000004E-2</v>
       </c>
       <c r="F43" s="11">
-        <v>2.01E-2</v>
+        <v>4.9900000000000007E-2</v>
       </c>
       <c r="G43" s="11">
-        <v>1.49E-2</v>
+        <v>6.4799999999999996E-2</v>
       </c>
       <c r="H43" s="11">
-        <v>2.01E-2</v>
+        <v>-9.459999999999999E-2</v>
       </c>
       <c r="I43" s="7"/>
     </row>
@@ -2487,19 +2495,19 @@
         <v>1.15E-2</v>
       </c>
       <c r="D44" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>0.02</v>
       </c>
       <c r="E44" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>-8.5000000000000006E-3</v>
       </c>
       <c r="F44" s="11">
-        <v>1.15E-2</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="G44" s="11">
-        <v>8.5000000000000006E-3</v>
+        <v>3.7000000000000005E-2</v>
       </c>
       <c r="H44" s="11">
-        <v>1.15E-2</v>
+        <v>-5.4000000000000006E-2</v>
       </c>
       <c r="I44" s="7"/>
     </row>
@@ -2514,19 +2522,19 @@
         <v>8.0500000000000002E-2</v>
       </c>
       <c r="D45" s="11">
-        <v>5.9499999999999997E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="E45" s="11">
-        <v>5.9499999999999997E-2</v>
+        <v>-5.9500000000000011E-2</v>
       </c>
       <c r="F45" s="11">
-        <v>8.0500000000000002E-2</v>
+        <v>0.19950000000000001</v>
       </c>
       <c r="G45" s="11">
-        <v>5.9499999999999997E-2</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="H45" s="11">
-        <v>8.0500000000000002E-2</v>
+        <v>-0.378</v>
       </c>
       <c r="I45" s="7"/>
     </row>
@@ -2541,19 +2549,19 @@
         <v>4.5999999999999999E-2</v>
       </c>
       <c r="D46" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>0.08</v>
       </c>
       <c r="E46" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>-3.4000000000000002E-2</v>
       </c>
       <c r="F46" s="11">
-        <v>4.5999999999999999E-2</v>
+        <v>0.114</v>
       </c>
       <c r="G46" s="11">
-        <v>3.4000000000000002E-2</v>
+        <v>0.14800000000000002</v>
       </c>
       <c r="H46" s="11">
-        <v>4.5999999999999999E-2</v>
+        <v>-0.21600000000000003</v>
       </c>
       <c r="I46" s="7"/>
     </row>
@@ -2568,19 +2576,19 @@
         <v>4.8899999999999999E-2</v>
       </c>
       <c r="D47" s="11">
-        <v>3.61E-2</v>
+        <v>8.4999999999999992E-2</v>
       </c>
       <c r="E47" s="11">
-        <v>3.61E-2</v>
+        <v>-3.6099999999999993E-2</v>
       </c>
       <c r="F47" s="11">
-        <v>4.8899999999999999E-2</v>
+        <v>0.12109999999999999</v>
       </c>
       <c r="G47" s="11">
-        <v>3.61E-2</v>
+        <v>0.15719999999999998</v>
       </c>
       <c r="H47" s="11">
-        <v>4.8899999999999999E-2</v>
+        <v>-0.22939999999999997</v>
       </c>
       <c r="I47" s="7"/>
     </row>
@@ -2595,19 +2603,19 @@
         <v>2.3E-2</v>
       </c>
       <c r="D48" s="11">
-        <v>1.7000000000000001E-2</v>
+        <v>0.04</v>
       </c>
       <c r="E48" s="11">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F48" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="G48" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="H48" s="25" t="s">
-        <v>48</v>
+        <v>-1.7000000000000001E-2</v>
+      </c>
+      <c r="F48" s="11">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="G48" s="11">
+        <v>7.400000000000001E-2</v>
+      </c>
+      <c r="H48" s="11">
+        <v>-0.10800000000000001</v>
       </c>
       <c r="I48" s="7"/>
     </row>
@@ -2628,12 +2636,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M298"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2692,7 +2700,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2703,7 +2711,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -2714,7 +2722,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -2726,7 +2734,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="str">
         <f ca="1">"  write.table(test_in[,1],file="""&amp;variablesVerzeichnis&amp;"/test_out.txt"",sep=""\t"",row.names=FALSE,col.names=FALSE,quote=FALSE)"</f>
-        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20200210/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
+        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20210306/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2748,7 +2756,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -2760,7 +2768,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="str">
         <f ca="1">"png(filename="""&amp;variablesVerzeichnis&amp;"/testdiagram.png"")"</f>
-        <v>png(filename="unterverz/unterunterverz/20200210/testdiagram.png")</v>
+        <v>png(filename="unterverz/unterunterverz/20210306/testdiagram.png")</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -2771,7 +2779,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12"/>
       <c r="D12"/>
@@ -2782,7 +2790,7 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13"/>
       <c r="D13"/>
@@ -2820,7 +2828,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16"/>
       <c r="D16"/>
@@ -2831,7 +2839,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
@@ -2852,7 +2860,7 @@
       </c>
       <c r="C18" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20200210</v>
+        <v>unterverz/unterunterverz/20210306</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -2865,11 +2873,11 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C19" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20200210</v>
+        <v>unterverz/unterunterverz/20210306</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
@@ -2903,10 +2911,10 @@
     </row>
     <row r="22" spans="1:8" ht="191.25" x14ac:dyDescent="0.2">
       <c r="A22" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C22"/>
       <c r="E22"/>
@@ -2916,7 +2924,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="16" t="s">
         <v>9</v>
@@ -2959,7 +2967,7 @@
     <row r="26" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26" s="24" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C26"/>
       <c r="D26"/>
@@ -9052,12 +9060,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="eingabeToy"/>
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:L12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9070,7 +9078,7 @@
     <col min="9" max="16384" width="11.42578125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>20</v>
       </c>
@@ -9103,7 +9111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9136,7 +9144,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9167,10 +9175,10 @@
         <v>6</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9200,34 +9208,36 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5"/>
       <c r="J5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7"/>
       <c r="J7" s="4" t="s">
         <v>18</v>
       </c>
       <c r="K7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="O7" s="4"/>
+      <c r="P7" s="25"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8"/>
       <c r="C8" s="6"/>
       <c r="J8" s="4" t="s">
@@ -9236,8 +9246,10 @@
       <c r="K8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O8" s="4"/>
+      <c r="P8"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9"/>
       <c r="J9" s="3" t="s">
         <v>1</v>
@@ -9245,45 +9257,53 @@
       <c r="K9" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="O9" s="3"/>
+      <c r="P9" s="2"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10"/>
       <c r="J10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="K10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="O10" s="3"/>
+      <c r="P10"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11"/>
       <c r="J11" s="3" t="s">
         <v>5</v>
       </c>
       <c r="K11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="O11" s="3"/>
+      <c r="P11"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12"/>
       <c r="J12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="K12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="O12" s="3"/>
+      <c r="P12"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
@@ -9390,12 +9410,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9408,10 +9428,10 @@
   <sheetData>
     <row r="1" spans="1:12" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>20</v>
@@ -9440,10 +9460,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>42736</v>
@@ -9461,7 +9481,7 @@
         <v>0.1</v>
       </c>
       <c r="I2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J2" s="1">
         <v>3</v>
@@ -9475,7 +9495,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D3">
         <v>42737</v>
@@ -9493,7 +9513,7 @@
         <v>0.8</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" s="1">
         <v>3</v>
@@ -9507,7 +9527,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4">
         <v>42738</v>
@@ -9525,7 +9545,7 @@
         <v>5</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J4" s="1">
         <v>3</v>
@@ -9539,7 +9559,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -9567,7 +9587,7 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -9582,7 +9602,7 @@
         <v>0.1</v>
       </c>
       <c r="J9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K9">
         <v>3</v>
@@ -9593,7 +9613,7 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10">
         <v>68.56</v>
@@ -9608,7 +9628,7 @@
         <v>0.8</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K10" s="22">
         <v>3</v>
@@ -9619,7 +9639,7 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F11">
         <v>300</v>
@@ -9634,7 +9654,7 @@
         <v>5</v>
       </c>
       <c r="J11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="K11" s="22">
         <v>3</v>
@@ -9648,18 +9668,18 @@
     </row>
     <row r="39" spans="1:2" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
@@ -9667,11 +9687,10 @@
         <v>7</v>
       </c>
       <c r="B41" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
log into Ribbon Menu tested Rdotnet, crashes with R>4.0.0 update to nuget MS packages
</commit_message>
<xml_diff>
--- a/test/testRAddin.xlsx
+++ b/test/testRAddin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\RAddin\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA0AFC1-6F4B-4EFA-8B59-C610759C3409}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D64C5C2A-03DC-4C6D-BCF3-89B16DC415A5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main Test" sheetId="1" r:id="rId1"/>
@@ -308,25 +308,6 @@
     <t>/c</t>
   </si>
   <si>
-    <t># cannot be called via shell, because test_in is not read from file -&gt; in memory !!
-library(ggplot2)
-test_out &lt;- as.Date(c("2017-01-01","2017-01-02","2017-01-03"))+25569 # difference between 1/1/1900 and 1/1/1970 + MS error
-test_out2 &lt;- test_in
-rownames(test_out2) &lt;- c("huey","dewey","louie")
-gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
-png(filename="C:/dev/Raddin/trunk/test/testdiagram.png")
-print(gplot)
-dev.off()</t>
-  </si>
-  <si>
-    <t># cannot be called via shell, because test_in is not read from file -&gt; in memory !!
-library(ggplot2)
-gplot &lt;- ggplot(data = test_in, aes(x = in6, y = in7) ) + geom_point()
-png(filename="C:/dev/Raddin/trunk/test/testdiagram.png")
-print(gplot)
-dev.off()</t>
-  </si>
-  <si>
     <t>if (length(script.basename) &gt; 0) {</t>
   </si>
   <si>
@@ -354,6 +335,25 @@
   </si>
   <si>
     <t>gplot &lt;- ggplot(data = test_in, aes(x = in5, y = in6) ) + geom_point()</t>
+  </si>
+  <si>
+    <t># cannot be called via shell, because test_in is not read from file -&gt; in memory !!
+library(ggplot2)
+test_out &lt;- as.Date(c("2017-01-01","2017-01-02","2017-01-03"))+25569 # difference between 1/1/1900 and 1/1/1970 + MS error
+test_out2 &lt;- test_in
+rownames(test_out2) &lt;- c("huey","dewey","louie")
+gplot &lt;- ggplot(data = test_in, aes(x = in1, y = in2) ) + geom_point()
+png(filename="C:/dev/Raddin/test/testdiagram.png")
+print(gplot)
+dev.off()</t>
+  </si>
+  <si>
+    <t># cannot be called via shell, because test_in is not read from file -&gt; in memory !!
+library(ggplot2)
+gplot &lt;- ggplot(data = test_in, aes(x = in6, y = in7) ) + geom_point()
+png(filename="C:/dev/Raddin/test/testdiagram.png")
+print(gplot)
+dev.off()</t>
   </si>
 </sst>
 </file>
@@ -747,6 +747,61 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>3810000</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="testdiagram.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB43D5FC-77F6-454E-801E-DA8FD6344F52}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="2409825"/>
+          <a:ext cx="4572000" cy="4572000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
@@ -1308,7 +1363,7 @@
       </c>
       <c r="U4" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210306</v>
+        <v>unterverz/unterunterverz/20210307</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
@@ -1369,7 +1424,7 @@
       </c>
       <c r="U5" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210306</v>
+        <v>unterverz/unterunterverz/20210307</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -1433,7 +1488,7 @@
       <c r="M7" s="7"/>
       <c r="U7" s="22" t="str">
         <f ca="1">"unterverz/unterunterverz/"&amp;TEXT(TODAY(),"JJJJMMTT")</f>
-        <v>unterverz/unterunterverz/20210306</v>
+        <v>unterverz/unterunterverz/20210307</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -2700,7 +2755,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5"/>
       <c r="D5"/>
@@ -2711,7 +2766,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B6" s="9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6"/>
       <c r="D6"/>
@@ -2722,7 +2777,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B7" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7"/>
       <c r="D7"/>
@@ -2734,7 +2789,7 @@
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="str">
         <f ca="1">"  write.table(test_in[,1],file="""&amp;variablesVerzeichnis&amp;"/test_out.txt"",sep=""\t"",row.names=FALSE,col.names=FALSE,quote=FALSE)"</f>
-        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20210306/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
+        <v xml:space="preserve">  write.table(test_in[,1],file="unterverz/unterunterverz/20210307/test_out.txt",sep="\t",row.names=FALSE,col.names=FALSE,quote=FALSE)</v>
       </c>
       <c r="C8"/>
       <c r="D8"/>
@@ -2756,7 +2811,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C10"/>
       <c r="D10"/>
@@ -2768,7 +2823,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="str">
         <f ca="1">"png(filename="""&amp;variablesVerzeichnis&amp;"/testdiagram.png"")"</f>
-        <v>png(filename="unterverz/unterunterverz/20210306/testdiagram.png")</v>
+        <v>png(filename="unterverz/unterunterverz/20210307/testdiagram.png")</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -2860,7 +2915,7 @@
       </c>
       <c r="C18" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210306</v>
+        <v>unterverz/unterunterverz/20210307</v>
       </c>
       <c r="D18"/>
       <c r="E18"/>
@@ -2877,7 +2932,7 @@
       </c>
       <c r="C19" t="str">
         <f ca="1">variablesVerzeichnis</f>
-        <v>unterverz/unterunterverz/20210306</v>
+        <v>unterverz/unterunterverz/20210307</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
@@ -2914,7 +2969,7 @@
         <v>40</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C22"/>
       <c r="E22"/>
@@ -9064,7 +9119,7 @@
   <sheetPr codeName="eingabeToy"/>
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
@@ -9414,8 +9469,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -9431,7 +9486,7 @@
         <v>40</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>20</v>
@@ -9671,7 +9726,7 @@
         <v>40</v>
       </c>
       <c r="B39" s="20" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
@@ -9692,5 +9747,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>